<commit_message>
Fix bill calculation and update discount handling in order management UI
</commit_message>
<xml_diff>
--- a/Backup/Order_Items.xlsx
+++ b/Backup/Order_Items.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1653,6 +1653,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>19</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CAND234</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1793.72197309417</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>